<commit_message>
C42203 committed with latest changes
</commit_message>
<xml_diff>
--- a/Testdata/Non_Oncology/DataFiles/ManageAbbreviations/LIVEHTA_3750_manageAbbreviation_Data.xlsx
+++ b/Testdata/Non_Oncology/DataFiles/ManageAbbreviations/LIVEHTA_3750_manageAbbreviation_Data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PSE WORKSPACE\pse.autotest\Testdata\Non_Oncology\DataFiles\ManageAbbreviations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2896DB9D-181B-4600-A16F-1168F3046D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6E870B-6AB6-4738-A835-AA26C74BFBF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="datafile" sheetId="1" r:id="rId1"/>
+    <sheet name="population0data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,9 +36,6 @@
     <t>Abbreviation</t>
   </si>
   <si>
-    <t xml:space="preserve">TestCytel - automation_nononcology </t>
-  </si>
-  <si>
     <t>Non-Oncology</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>Real-world Evidence</t>
+  </si>
+  <si>
+    <t>TestCytel - automation_nononcology</t>
   </si>
 </sst>
 </file>
@@ -399,7 +399,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -414,7 +414,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -426,54 +426,54 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>